<commit_message>
Ended V2 of algorythm
</commit_message>
<xml_diff>
--- a/JeuDonneesWorkshop23.xlsx
+++ b/JeuDonneesWorkshop23.xlsx
@@ -1,18 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\courb\iCloudDrive\MASTER EII - 2nd année\1 - WorkShop\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7EC81EB-DE21-4C2A-A898-993FC2447138}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="patient" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="Durée des soins" sheetId="2" r:id="rId5"/>
+    <sheet name="patient" sheetId="1" r:id="rId1"/>
+    <sheet name="Durée des soins" sheetId="2" r:id="rId2"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="42">
   <si>
     <t>Soins</t>
   </si>
@@ -135,26 +144,31 @@
   </si>
   <si>
     <t>Piqûre</t>
+  </si>
+  <si>
+    <t>15 rue de celloville 76240 Belbeuf</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
@@ -165,43 +179,44 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -391,319 +406,359 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:F16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="28.28515625" customWidth="1"/>
+    <col min="4" max="4" width="21.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="A2:A16" xr:uid="{00000000-0002-0000-0000-000000000000}">
+      <formula1>"Piqûre    ,Repas,Elimination,Pansement,Lavage"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
-  <cols>
-    <col customWidth="1" min="1" max="1" width="28.25"/>
-    <col customWidth="1" min="4" max="4" width="21.5"/>
-  </cols>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2">
+      <c r="B1" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="2" t="s">
+      <c r="B6" s="2">
         <v>15</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>9</v>
-      </c>
     </row>
   </sheetData>
-  <dataValidations>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="A2:A15">
-      <formula1>"Piqûre    ,Repas,Elimination,Pansement,Lavage"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B2" s="2">
-        <v>10.0</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3" s="2">
-        <v>30.0</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B4" s="2">
-        <v>15.0</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B5" s="2">
-        <v>20.0</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="2">
-        <v>15.0</v>
-      </c>
-    </row>
-  </sheetData>
-  <drawing r:id="rId1"/>
-</worksheet>
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="d89bc650-3cd4-470c-8e9f-01e18e5de623">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="de834f96-3fa5-4532-8779-e3fc16ae52f9" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010000DFD5B32E7AAD4E87CF33AB4C50A6F6" ma:contentTypeVersion="11" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="36a8408312e9b7bebfe6e96aa03e94e5">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="d89bc650-3cd4-470c-8e9f-01e18e5de623" xmlns:ns3="de834f96-3fa5-4532-8779-e3fc16ae52f9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2ad024853857a5ece2a89d98fa5e6952" ns2:_="" ns3:_="">
     <xsd:import namespace="d89bc650-3cd4-470c-8e9f-01e18e5de623"/>
@@ -912,34 +967,40 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BF73415B-66E5-4DA0-837C-9DE170B0CFE8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="d89bc650-3cd4-470c-8e9f-01e18e5de623"/>
+    <ds:schemaRef ds:uri="de834f96-3fa5-4532-8779-e3fc16ae52f9"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="d89bc650-3cd4-470c-8e9f-01e18e5de623">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="de834f96-3fa5-4532-8779-e3fc16ae52f9" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4883A9A4-BC98-4CA1-BB1C-4E2981A09AE2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DF57347C-2E8A-453E-8DEA-18C460D82A55}"/>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4883A9A4-BC98-4CA1-BB1C-4E2981A09AE2}"/>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BF73415B-66E5-4DA0-837C-9DE170B0CFE8}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DF57347C-2E8A-453E-8DEA-18C460D82A55}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="d89bc650-3cd4-470c-8e9f-01e18e5de623"/>
+    <ds:schemaRef ds:uri="de834f96-3fa5-4532-8779-e3fc16ae52f9"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>